<commit_message>
Updated status of my user stories
</commit_message>
<xml_diff>
--- a/docs/Team01Report-Sprint2.xlsx
+++ b/docs/Team01Report-Sprint2.xlsx
@@ -333,213 +333,219 @@
     <t>Birth before death of parents</t>
   </si>
   <si>
+    <t>US21</t>
+  </si>
+  <si>
+    <t>Correct gender for role</t>
+  </si>
+  <si>
+    <t>The goal of the burndown chart is to help the agile team and customer to understand how the developers are doing</t>
+  </si>
+  <si>
+    <t>to deliver the product.  Burndown charts can be done daily, weekly, at the end of a sprint, or at whatever time interval makes sense.</t>
+  </si>
+  <si>
+    <t>We'll update our burndown chart for the GEDCOM project at the end of each sprint.</t>
+  </si>
+  <si>
+    <t>At the end of each sprint, you should update the number of remaining stories, the LOC written to implement the user stories</t>
+  </si>
+  <si>
+    <t>implemented in this sprint, and the minutes needed to write those lines of code.</t>
+  </si>
+  <si>
+    <t>Here's a sample burndown chart for a team of three:</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Remaining Stories</t>
+  </si>
+  <si>
+    <t>Story Velocity</t>
+  </si>
+  <si>
+    <t>LOC</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Code Velocity</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>Est Size</t>
+  </si>
+  <si>
+    <t>Est Time</t>
+  </si>
+  <si>
+    <t>Act Size</t>
+  </si>
+  <si>
+    <t>Act Time</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>T04.01</t>
+  </si>
+  <si>
+    <t>Store Marriage Date</t>
+  </si>
+  <si>
+    <t>Store Divorce date</t>
+  </si>
+  <si>
+    <t>T10.01</t>
+  </si>
+  <si>
+    <t>Store age</t>
+  </si>
+  <si>
+    <t>T22.01</t>
+  </si>
+  <si>
+    <t>Store IDs</t>
+  </si>
+  <si>
+    <t>Compare</t>
+  </si>
+  <si>
+    <t>T03.01</t>
+  </si>
+  <si>
+    <t>Store dates</t>
+  </si>
+  <si>
+    <t>Validate</t>
+  </si>
+  <si>
+    <t>coding</t>
+  </si>
+  <si>
+    <t>US28</t>
+  </si>
+  <si>
+    <t>Order siblings by age</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>CODING</t>
+  </si>
+  <si>
+    <t>US35</t>
+  </si>
+  <si>
+    <t>List recent births</t>
+  </si>
+  <si>
+    <t>US30</t>
+  </si>
+  <si>
+    <t>List living married</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>US31</t>
+  </si>
+  <si>
+    <t>List living single</t>
+  </si>
+  <si>
+    <t>US32</t>
+  </si>
+  <si>
+    <t>List multiple births</t>
+  </si>
+  <si>
+    <t>VK</t>
+  </si>
+  <si>
+    <t>US37</t>
+  </si>
+  <si>
+    <t>List recent survivors</t>
+  </si>
+  <si>
+    <t>US41</t>
+  </si>
+  <si>
+    <t>Include partial dates</t>
+  </si>
+  <si>
+    <t>SK</t>
+  </si>
+  <si>
+    <t>US42</t>
+  </si>
+  <si>
+    <t>Reject illegitimate dates</t>
+  </si>
+  <si>
+    <t>Story Description</t>
+  </si>
+  <si>
+    <t>US01</t>
+  </si>
+  <si>
+    <t>Dates before current date</t>
+  </si>
+  <si>
+    <t>Dates (birth, marriage, divorce, death) should not be after the current date</t>
+  </si>
+  <si>
+    <t>US02</t>
+  </si>
+  <si>
+    <t>Birth should occur before marriage of an individual</t>
+  </si>
+  <si>
+    <t>Birth before death</t>
+  </si>
+  <si>
+    <t>Birth should occur before death of an individual</t>
+  </si>
+  <si>
+    <t>Marriage should occur before divorce of spouses, and divorce can only occur after marriage</t>
+  </si>
+  <si>
+    <t>US05</t>
+  </si>
+  <si>
+    <t>Marriage should occur before death of either spouse</t>
+  </si>
+  <si>
     <t>US06</t>
   </si>
   <si>
     <t>Divorce before death</t>
   </si>
   <si>
-    <t>The goal of the burndown chart is to help the agile team and customer to understand how the developers are doing</t>
-  </si>
-  <si>
-    <t>to deliver the product.  Burndown charts can be done daily, weekly, at the end of a sprint, or at whatever time interval makes sense.</t>
-  </si>
-  <si>
-    <t>We'll update our burndown chart for the GEDCOM project at the end of each sprint.</t>
-  </si>
-  <si>
-    <t>At the end of each sprint, you should update the number of remaining stories, the LOC written to implement the user stories</t>
-  </si>
-  <si>
-    <t>implemented in this sprint, and the minutes needed to write those lines of code.</t>
-  </si>
-  <si>
-    <t>Here's a sample burndown chart for a team of three:</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Remaining Stories</t>
-  </si>
-  <si>
-    <t>Story Velocity</t>
-  </si>
-  <si>
-    <t>LOC</t>
-  </si>
-  <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>Code Velocity</t>
-  </si>
-  <si>
-    <t>Start</t>
-  </si>
-  <si>
-    <t>Sprint 1</t>
-  </si>
-  <si>
-    <t>Sprint 2</t>
-  </si>
-  <si>
-    <t>Sprint 3</t>
-  </si>
-  <si>
-    <t>Sprint 4</t>
-  </si>
-  <si>
-    <t>Est Size</t>
-  </si>
-  <si>
-    <t>Est Time</t>
-  </si>
-  <si>
-    <t>Act Size</t>
-  </si>
-  <si>
-    <t>Act Time</t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>T04.01</t>
-  </si>
-  <si>
-    <t>Store Marriage Date</t>
-  </si>
-  <si>
-    <t>Store Divorce date</t>
-  </si>
-  <si>
-    <t>T10.01</t>
-  </si>
-  <si>
-    <t>Store age</t>
-  </si>
-  <si>
-    <t>T22.01</t>
-  </si>
-  <si>
-    <t>Store IDs</t>
-  </si>
-  <si>
-    <t>Compare</t>
-  </si>
-  <si>
-    <t>T03.01</t>
-  </si>
-  <si>
-    <t>Store dates</t>
-  </si>
-  <si>
-    <t>Validate</t>
-  </si>
-  <si>
-    <t>coding</t>
-  </si>
-  <si>
-    <t>US28</t>
-  </si>
-  <si>
-    <t>Order siblings by age</t>
-  </si>
-  <si>
-    <t>TC</t>
-  </si>
-  <si>
-    <t>CODING</t>
-  </si>
-  <si>
-    <t>US35</t>
-  </si>
-  <si>
-    <t>List recent births</t>
-  </si>
-  <si>
-    <t>US30</t>
-  </si>
-  <si>
-    <t>List living married</t>
-  </si>
-  <si>
-    <t>ST</t>
-  </si>
-  <si>
-    <t>US31</t>
-  </si>
-  <si>
-    <t>List living single</t>
-  </si>
-  <si>
-    <t>US32</t>
-  </si>
-  <si>
-    <t>List multiple births</t>
-  </si>
-  <si>
-    <t>VK</t>
-  </si>
-  <si>
-    <t>US37</t>
-  </si>
-  <si>
-    <t>List recent survivors</t>
-  </si>
-  <si>
-    <t>US41</t>
-  </si>
-  <si>
-    <t>Include partial dates</t>
-  </si>
-  <si>
-    <t>SK</t>
-  </si>
-  <si>
-    <t>US42</t>
-  </si>
-  <si>
-    <t>Reject illegitimate dates</t>
-  </si>
-  <si>
-    <t>Story Description</t>
-  </si>
-  <si>
-    <t>US01</t>
-  </si>
-  <si>
-    <t>Dates before current date</t>
-  </si>
-  <si>
-    <t>Dates (birth, marriage, divorce, death) should not be after the current date</t>
-  </si>
-  <si>
-    <t>US02</t>
-  </si>
-  <si>
-    <t>Birth should occur before marriage of an individual</t>
-  </si>
-  <si>
-    <t>Birth before death</t>
-  </si>
-  <si>
-    <t>Birth should occur before death of an individual</t>
-  </si>
-  <si>
-    <t>Marriage should occur before divorce of spouses, and divorce can only occur after marriage</t>
-  </si>
-  <si>
-    <t>US05</t>
-  </si>
-  <si>
-    <t>Marriage should occur before death of either spouse</t>
-  </si>
-  <si>
     <t>Divorce can only occur before death of both spouses</t>
   </si>
   <si>
@@ -643,12 +649,6 @@
   </si>
   <si>
     <t>Aunts and uncles should not marry their nieces or nephews</t>
-  </si>
-  <si>
-    <t>US21</t>
-  </si>
-  <si>
-    <t>Correct gender for role</t>
   </si>
   <si>
     <t>Husband in family should be male and wife in family should be female</t>
@@ -842,7 +842,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="13"/>
+      <color indexed="12"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -872,7 +872,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -905,11 +905,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -918,7 +918,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -926,17 +926,17 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top/>
@@ -953,7 +953,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top/>
       <bottom/>
@@ -961,12 +961,23 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -975,59 +986,48 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1035,36 +1035,36 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1096,28 +1096,28 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1135,20 +1135,20 @@
     <xf numFmtId="49" fontId="4" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -1254,8 +1254,8 @@
       <rgbColor rgb="015e88b1"/>
       <rgbColor rgb="01eef3f4"/>
       <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff5e88b1"/>
       <rgbColor rgb="ffeef3f4"/>
       <rgbColor rgb="ffd6e3bc"/>
@@ -1278,10 +1278,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0833081"/>
-          <c:y val="0.0581198"/>
-          <c:w val="0.911692"/>
-          <c:h val="0.85673"/>
+          <c:x val="0.0473273"/>
+          <c:y val="0.0588556"/>
+          <c:w val="0.947673"/>
+          <c:h val="0.855075"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1308,7 +1308,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="diamond"/>
-            <c:size val="5"/>
+            <c:size val="4"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -1350,23 +1350,23 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Burndown'!$B$15:$B$20</c:f>
+              <c:f>'Sprint1'!$B$15:$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6/6/16</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6/19/16</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7/3/16</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7/17/16</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7/31/16</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -1376,24 +1376,9 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown'!$C$15:$C$20</c:f>
+              <c:f>'Sprint1'!$C$15:$C$20</c:f>
               <c:numCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>24.000000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>18.000000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.000000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.000000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.000000</c:v>
-                </c:pt>
+                <c:ptCount val="0"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1487,8 +1472,8 @@
         <c:crossAx val="2094734552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="7.5"/>
-        <c:minorUnit val="3.75"/>
+        <c:majorUnit val="1"/>
+        <c:minorUnit val="0.5"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -1532,10 +1517,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0851619"/>
-          <c:y val="0.0581199"/>
-          <c:w val="0.909838"/>
-          <c:h val="0.85673"/>
+          <c:x val="0.0484233"/>
+          <c:y val="0.0588556"/>
+          <c:w val="0.946577"/>
+          <c:h val="0.855075"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1562,7 +1547,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="diamond"/>
-            <c:size val="5"/>
+            <c:size val="4"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -1604,41 +1589,35 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint1'!$A$2:$A$7</c:f>
+              <c:f>'Sprint2'!$A$2:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2/13</c:v>
+                  <c:v>US04</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2/28</c:v>
+                  <c:v>T04.01</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>T04.01</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>US10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v/>
+                  <c:v>T10.01</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint1'!$B$2:$B$7</c:f>
+              <c:f>'Sprint2'!$B$2:$B$7</c:f>
               <c:numCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>36.000000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>31.000000</c:v>
-                </c:pt>
+                <c:ptCount val="0"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1732,8 +1711,8 @@
         <c:crossAx val="2094734552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="1.5"/>
-        <c:minorUnit val="0.75"/>
+        <c:majorUnit val="1"/>
+        <c:minorUnit val="0.5"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -1769,16 +1748,16 @@
 <xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>768821</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>119868</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>11641</xdr:rowOff>
+      <xdr:rowOff>11640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>243872</xdr:colOff>
+      <xdr:colOff>220652</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>43009</xdr:rowOff>
+      <xdr:rowOff>10230</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1786,8 +1765,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="768821" y="3573991"/>
-        <a:ext cx="4643952" cy="2622169"/>
+        <a:off x="945368" y="3573990"/>
+        <a:ext cx="4444185" cy="2589391"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1800,15 +1779,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>430952</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>43641</xdr:rowOff>
+      <xdr:colOff>401163</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>44321</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1154044</xdr:colOff>
+      <xdr:colOff>1173094</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>33537</xdr:rowOff>
+      <xdr:rowOff>129935</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -1817,10 +1796,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1256452" y="1177116"/>
-          <a:ext cx="1446993" cy="1285297"/>
-          <a:chOff x="0" y="-68770"/>
-          <a:chExt cx="1408892" cy="1117649"/>
+          <a:off x="1226663" y="1015871"/>
+          <a:ext cx="1495832" cy="1542940"/>
+          <a:chOff x="-10462" y="-56388"/>
+          <a:chExt cx="1457455" cy="1341685"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp>
@@ -1830,8 +1809,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="0" y="79086"/>
-            <a:ext cx="1408893" cy="969794"/>
+            <a:off x="0" y="170034"/>
+            <a:ext cx="1446993" cy="1115264"/>
           </a:xfrm>
           <a:custGeom>
             <a:avLst/>
@@ -1927,8 +1906,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="8361" y="-68771"/>
-            <a:ext cx="1219832" cy="1054480"/>
+            <a:off x="-10463" y="-56389"/>
+            <a:ext cx="1290920" cy="864612"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2050,15 +2029,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>75349</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>93972</xdr:rowOff>
+      <xdr:colOff>45648</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>134752</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>537633</xdr:colOff>
+      <xdr:colOff>567331</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>62914</xdr:rowOff>
+      <xdr:rowOff>133450</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -2067,10 +2046,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5244249" y="1227447"/>
-          <a:ext cx="1300485" cy="940493"/>
-          <a:chOff x="0" y="-44005"/>
-          <a:chExt cx="1262383" cy="817819"/>
+          <a:off x="5214548" y="1106302"/>
+          <a:ext cx="1359883" cy="1132174"/>
+          <a:chOff x="-10347" y="-44006"/>
+          <a:chExt cx="1321176" cy="984498"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp>
@@ -2080,8 +2059,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="0" y="64846"/>
-            <a:ext cx="1262384" cy="708968"/>
+            <a:off x="-1" y="125178"/>
+            <a:ext cx="1300487" cy="815315"/>
           </a:xfrm>
           <a:custGeom>
             <a:avLst/>
@@ -2177,8 +2156,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="8448" y="-44006"/>
-            <a:ext cx="1245485" cy="674750"/>
+            <a:off x="-10348" y="-44007"/>
+            <a:ext cx="1321178" cy="674748"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2249,15 +2228,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1201420</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>51109</xdr:rowOff>
+      <xdr:colOff>1171888</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>53381</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>156635</xdr:colOff>
+      <xdr:colOff>186163</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>19778</xdr:rowOff>
+      <xdr:rowOff>114584</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -2266,10 +2245,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2750820" y="1022659"/>
-          <a:ext cx="1101516" cy="1264070"/>
-          <a:chOff x="0" y="-56389"/>
-          <a:chExt cx="1063415" cy="1099189"/>
+          <a:off x="2721288" y="863006"/>
+          <a:ext cx="1160576" cy="1518529"/>
+          <a:chOff x="-10131" y="-56388"/>
+          <a:chExt cx="1121775" cy="1320459"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp>
@@ -2279,8 +2258,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="0" y="64845"/>
-            <a:ext cx="1063416" cy="977956"/>
+            <a:off x="0" y="139419"/>
+            <a:ext cx="1101516" cy="1124652"/>
           </a:xfrm>
           <a:custGeom>
             <a:avLst/>
@@ -2376,8 +2355,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="8610" y="-56390"/>
-            <a:ext cx="1046193" cy="864615"/>
+            <a:off x="-10132" y="-56389"/>
+            <a:ext cx="1121776" cy="864612"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2448,15 +2427,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>115568</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>45231</xdr:rowOff>
+      <xdr:colOff>96518</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>97853</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>24130</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>67987</xdr:rowOff>
+      <xdr:colOff>43180</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>76909</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -2465,10 +2444,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3811268" y="1340631"/>
-          <a:ext cx="429263" cy="994307"/>
-          <a:chOff x="0" y="-56387"/>
-          <a:chExt cx="391161" cy="864613"/>
+          <a:off x="3792218" y="1231328"/>
+          <a:ext cx="467363" cy="950607"/>
+          <a:chOff x="0" y="-44005"/>
+          <a:chExt cx="429262" cy="826614"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp>
@@ -2478,8 +2457,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="0" y="79086"/>
-            <a:ext cx="391162" cy="545055"/>
+            <a:off x="0" y="155795"/>
+            <a:ext cx="429263" cy="626815"/>
           </a:xfrm>
           <a:custGeom>
             <a:avLst/>
@@ -2575,8 +2554,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="19780" y="-56388"/>
-            <a:ext cx="351600" cy="864614"/>
+            <a:off x="2656" y="-44006"/>
+            <a:ext cx="423948" cy="674748"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2698,15 +2677,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>502920</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>59905</xdr:rowOff>
+      <xdr:colOff>473334</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>56521</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>186267</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>103984</xdr:rowOff>
+      <xdr:colOff>215850</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>42521</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -2715,10 +2694,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4198620" y="1031455"/>
-          <a:ext cx="1156548" cy="1339480"/>
-          <a:chOff x="0" y="-56387"/>
-          <a:chExt cx="1118447" cy="1164763"/>
+          <a:off x="4169034" y="866146"/>
+          <a:ext cx="1215717" cy="1605251"/>
+          <a:chOff x="-10199" y="-56388"/>
+          <a:chExt cx="1176944" cy="1395868"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp>
@@ -2728,8 +2707,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="-1" y="64846"/>
-            <a:ext cx="1118449" cy="1043531"/>
+            <a:off x="-2" y="139418"/>
+            <a:ext cx="1156550" cy="1200063"/>
           </a:xfrm>
           <a:custGeom>
             <a:avLst/>
@@ -2825,8 +2804,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="8559" y="-56388"/>
-            <a:ext cx="1101328" cy="864614"/>
+            <a:off x="-10200" y="-56389"/>
+            <a:ext cx="1176945" cy="864612"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2897,15 +2876,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>206842</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>79971</xdr:rowOff>
+      <xdr:colOff>187792</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>100687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>664631</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>154509</xdr:rowOff>
+      <xdr:colOff>694326</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>83186</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -2914,10 +2893,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5375742" y="4775796"/>
-          <a:ext cx="1295990" cy="1208014"/>
-          <a:chOff x="0" y="-44005"/>
-          <a:chExt cx="1257889" cy="1050445"/>
+          <a:off x="5356692" y="4634587"/>
+          <a:ext cx="1344735" cy="1439825"/>
+          <a:chOff x="0" y="-44006"/>
+          <a:chExt cx="1306330" cy="1252020"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp>
@@ -2927,8 +2906,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="0" y="64846"/>
-            <a:ext cx="1257890" cy="941595"/>
+            <a:off x="0" y="125178"/>
+            <a:ext cx="1295990" cy="1082837"/>
           </a:xfrm>
           <a:custGeom>
             <a:avLst/>
@@ -3024,8 +3003,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="30013" y="-44006"/>
-            <a:ext cx="1219424" cy="674750"/>
+            <a:off x="11872" y="-44007"/>
+            <a:ext cx="1294459" cy="674748"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -3100,16 +3079,16 @@
 <xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>768820</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>119867</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>11642</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>244382</xdr:colOff>
+      <xdr:colOff>221667</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>43009</xdr:rowOff>
+      <xdr:rowOff>10231</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3117,8 +3096,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="768820" y="1468967"/>
-        <a:ext cx="4542863" cy="2622168"/>
+        <a:off x="945367" y="1468967"/>
+        <a:ext cx="4343601" cy="2589390"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4220,7 +4199,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -4478,16 +4457,19 @@
       <c r="D26" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="E26" s="24"/>
-    </row>
-    <row r="27">
+      <c r="E26" s="21"/>
+    </row>
+    <row r="27" ht="13" customHeight="1">
+      <c r="A27" s="7"/>
       <c r="B27" t="s" s="3">
         <v>22</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-    </row>
-    <row r="28">
+      <c r="E27" s="9"/>
+    </row>
+    <row r="28" ht="13" customHeight="1">
+      <c r="A28" s="20"/>
       <c r="B28" s="4"/>
       <c r="C28" t="s" s="4">
         <v>5</v>
@@ -4495,6 +4477,7 @@
       <c r="D28" t="s" s="5">
         <v>22</v>
       </c>
+      <c r="E28" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4504,14 +4487,15 @@
   <hyperlinks>
     <hyperlink ref="D10" location="'Export Summary'!R1C1" tooltip="" display="Export Summary"/>
     <hyperlink ref="D10" location="'Team'!R1C1" tooltip="" display="Team"/>
-    <hyperlink ref="D12" location="'Backlog'!R1C1" tooltip="" display="Backlog"/>
-    <hyperlink ref="D14" location="'Burndown README'!R1C1" tooltip="" display="Burndown README"/>
-    <hyperlink ref="D16" location="'Burndown'!R1C1" tooltip="" display="Burndown"/>
-    <hyperlink ref="D18" location="'Sprint1'!R1C1" tooltip="" display="Sprint1"/>
-    <hyperlink ref="D20" location="'Sprint2'!R1C1" tooltip="" display="Sprint2"/>
-    <hyperlink ref="D22" location="'Sprint3'!R1C1" tooltip="" display="Sprint3"/>
-    <hyperlink ref="D24" location="'Sprint4'!R1C1" tooltip="" display="Sprint4"/>
-    <hyperlink ref="D26" location="'Stories'!R1C1" tooltip="" display="Stories"/>
+    <hyperlink ref="D12" location="'Team'!R1C1" tooltip="" display="Team"/>
+    <hyperlink ref="D14" location="'Backlog'!R1C1" tooltip="" display="Backlog"/>
+    <hyperlink ref="D16" location="'Burndown README'!R1C1" tooltip="" display="Burndown README"/>
+    <hyperlink ref="D18" location="'Burndown'!R1C1" tooltip="" display="Burndown"/>
+    <hyperlink ref="D20" location="'Sprint1'!R1C1" tooltip="" display="Sprint1"/>
+    <hyperlink ref="D22" location="'Sprint2'!R1C1" tooltip="" display="Sprint2"/>
+    <hyperlink ref="D24" location="'Sprint3'!R1C1" tooltip="" display="Sprint3"/>
+    <hyperlink ref="D26" location="'Sprint4'!R1C1" tooltip="" display="Sprint4"/>
+    <hyperlink ref="D28" location="'Stories'!R1C1" tooltip="" display="Stories"/>
     <hyperlink ref="D12" location="'Team'!R1C1" tooltip="" display="Team"/>
     <hyperlink ref="D14" location="'Backlog'!R1C1" tooltip="" display="Backlog"/>
     <hyperlink ref="D16" location="'Burndown README'!R1C1" tooltip="" display="Burndown README"/>
@@ -4625,13 +4609,13 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" t="s" s="26">
-        <v>77</v>
+        <v>146</v>
       </c>
       <c r="B7" t="s" s="26">
-        <v>78</v>
+        <v>147</v>
       </c>
       <c r="C7" t="s" s="52">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="27"/>
@@ -4644,7 +4628,7 @@
         <v>71</v>
       </c>
       <c r="C8" t="s" s="52">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D8" s="27"/>
       <c r="E8" s="27"/>
@@ -4657,7 +4641,7 @@
         <v>74</v>
       </c>
       <c r="C9" t="s" s="52">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D9" s="27"/>
       <c r="E9" s="27"/>
@@ -4670,7 +4654,7 @@
         <v>76</v>
       </c>
       <c r="C10" t="s" s="52">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D10" s="27"/>
       <c r="E10" s="27"/>
@@ -4683,147 +4667,147 @@
         <v>56</v>
       </c>
       <c r="C11" t="s" s="52">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="27"/>
     </row>
     <row r="12" ht="31.5" customHeight="1">
       <c r="A12" t="s" s="26">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B12" t="s" s="26">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C12" t="s" s="52">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D12" s="27"/>
       <c r="E12" s="27"/>
     </row>
     <row r="13" ht="47.25" customHeight="1">
       <c r="A13" t="s" s="26">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B13" t="s" s="26">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C13" t="s" s="52">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D13" s="27"/>
       <c r="E13" s="27"/>
     </row>
     <row r="14" ht="63" customHeight="1">
       <c r="A14" t="s" s="26">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B14" t="s" s="26">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C14" t="s" s="52">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D14" s="27"/>
       <c r="E14" s="27"/>
     </row>
     <row r="15" ht="31.5" customHeight="1">
       <c r="A15" t="s" s="26">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B15" t="s" s="26">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C15" t="s" s="52">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D15" s="27"/>
       <c r="E15" s="27"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" t="s" s="26">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B16" t="s" s="26">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C16" t="s" s="52">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D16" s="27"/>
       <c r="E16" s="27"/>
     </row>
     <row r="17" ht="31.5" customHeight="1">
       <c r="A17" t="s" s="26">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B17" t="s" s="26">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C17" t="s" s="52">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D17" s="27"/>
       <c r="E17" s="27"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" t="s" s="26">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B18" t="s" s="26">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C18" t="s" s="52">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D18" s="27"/>
       <c r="E18" s="27"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" t="s" s="26">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B19" t="s" s="26">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C19" t="s" s="52">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D19" s="27"/>
       <c r="E19" s="27"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" t="s" s="26">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B20" t="s" s="26">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C20" t="s" s="52">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D20" s="27"/>
       <c r="E20" s="27"/>
     </row>
     <row r="21" ht="31.5" customHeight="1">
       <c r="A21" t="s" s="26">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B21" t="s" s="26">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C21" t="s" s="52">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D21" s="27"/>
       <c r="E21" s="27"/>
     </row>
     <row r="22" ht="31.5" customHeight="1">
       <c r="A22" t="s" s="26">
-        <v>181</v>
+        <v>77</v>
       </c>
       <c r="B22" t="s" s="26">
-        <v>182</v>
+        <v>78</v>
       </c>
       <c r="C22" t="s" s="52">
         <v>183</v>

</xml_diff>